<commit_message>
Update Q&A, Update UC Admin
</commit_message>
<xml_diff>
--- a/Docs/Q&A/DD_RFID_Q&A_v1.0.xlsx
+++ b/Docs/Q&A/DD_RFID_Q&A_v1.0.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>Notes</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -456,74 +456,6 @@
   </si>
   <si>
     <t>Deadline for a reply. Filled in by FPT</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <t>Open:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> The question has not been answered </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Closed:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> The question is satisfactorily answered</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Canceled:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Question is canceled
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">In progress: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>the answer is available but not fully satisfied</t>
-    </r>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -678,12 +610,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>Có thể dùng loại đầu đọc giống niên luận và dùng laravel để xây dựng web được không ạ?</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -691,6 +617,91 @@
   </si>
   <si>
     <t>Confirmation</t>
+  </si>
+  <si>
+    <t>Xác nhận thiết bị sử dụng</t>
+  </si>
+  <si>
+    <t>Loại file xuất ra</t>
+  </si>
+  <si>
+    <t>Các chức năng xuất file xuất ra file dạng nào?</t>
+  </si>
+  <si>
+    <t>Có thể dùng loại đầu đọc giống niên luận và dùng laravel để xây dựng web được không?</t>
+  </si>
+  <si>
+    <t>Danh sách vắng (không có vào theo toàn thể danh sách SV/CB) có phải là danh sách những người không đăng kí tham gia không?</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <r>
+      <t>Open:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The question has not been answered </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Closed:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The question is satisfactorily answered</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Canceled:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Question is canceled
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">In progress: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>the answer is available but not fully satisfied</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1051,6 +1062,24 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1088,50 +1117,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1612,78 +1602,78 @@
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="22"/>
@@ -1726,9 +1716,9 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I13" sqref="I13"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1740,26 +1730,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="42"/>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:2" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="20"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1780,15 +1770,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>8</v>
@@ -1801,7 +1791,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>10</v>
@@ -1828,7 +1818,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1837,7 +1827,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1877,7 +1867,7 @@
         <v>45</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="140.25" x14ac:dyDescent="0.2">
@@ -1885,7 +1875,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
@@ -1925,7 +1915,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1962,10 +1952,10 @@
     </row>
     <row r="34" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1997,7 +1987,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2012,8 +2002,8 @@
     <col min="8" max="8" width="11.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="11" style="3" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="20" style="41" customWidth="1"/>
-    <col min="12" max="12" width="17" style="41" customWidth="1"/>
+    <col min="11" max="11" width="20" style="26" customWidth="1"/>
+    <col min="12" max="12" width="17" style="26" customWidth="1"/>
     <col min="13" max="13" width="17" style="3" customWidth="1"/>
     <col min="14" max="15" width="20.42578125" style="3" customWidth="1"/>
     <col min="16" max="16" width="22.42578125" style="3" customWidth="1"/>
@@ -2021,53 +2011,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="43"/>
       <c r="C1" s="3">
         <f>COUNTIF(J:J, "Open")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="3">
         <f>COUNTIF(J:J, "In progress")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="39"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="3">
         <f>COUNTIF(J:J, "Closed")</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="3">
         <f>COUNTIF(J:J, "Canceled")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="40"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="3">
         <f>SUM(C1:C4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2081,10 +2071,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>3</v>
@@ -2101,10 +2091,10 @@
       <c r="J7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="27" t="s">
         <v>6</v>
       </c>
       <c r="M7" s="4" t="s">
@@ -2114,130 +2104,164 @@
         <v>20</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44">
+      <c r="A8" s="29">
         <v>1</v>
       </c>
-      <c r="B8" s="44" t="s">
-        <v>72</v>
+      <c r="B8" s="29" t="s">
+        <v>71</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>73</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="H8" s="21"/>
       <c r="I8" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="43">
+        <v>86</v>
+      </c>
+      <c r="K8" s="28">
         <v>42925</v>
       </c>
-      <c r="L8" s="43">
+      <c r="L8" s="28">
         <f>K8+7</f>
         <v>42932</v>
       </c>
       <c r="M8" s="25"/>
       <c r="N8" s="6"/>
       <c r="O8" s="21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:16" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44">
+      <c r="A9" s="29">
         <v>2</v>
       </c>
-      <c r="B9" s="44" t="s">
-        <v>72</v>
+      <c r="B9" s="29" t="s">
+        <v>71</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="E9" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>73</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="H9" s="21"/>
       <c r="I9" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K9" s="43">
+        <v>86</v>
+      </c>
+      <c r="K9" s="28">
         <v>42925</v>
       </c>
-      <c r="L9" s="43">
+      <c r="L9" s="28">
         <f t="shared" ref="L9:L11" si="0">K9+7</f>
         <v>42932</v>
       </c>
       <c r="M9" s="25"/>
       <c r="N9" s="6"/>
       <c r="O9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:16" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29">
+        <v>3</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="44">
-        <v>3</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="46"/>
+      <c r="G10" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="30">
+        <v>42925</v>
+      </c>
+      <c r="L10" s="28">
+        <f t="shared" si="0"/>
+        <v>42932</v>
+      </c>
+      <c r="M10" s="31"/>
       <c r="N10" s="6"/>
-      <c r="O10" s="44"/>
+      <c r="O10" s="29" t="s">
+        <v>79</v>
+      </c>
       <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:16" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="44">
+      <c r="A11" s="29">
         <v>4</v>
       </c>
-      <c r="B11" s="44"/>
+      <c r="B11" s="29" t="s">
+        <v>71</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="46"/>
+      <c r="G11" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" s="30">
+        <v>42925</v>
+      </c>
+      <c r="L11" s="30">
+        <f t="shared" si="0"/>
+        <v>42932</v>
+      </c>
+      <c r="M11" s="31"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="44"/>
+      <c r="O11" s="29" t="s">
+        <v>79</v>
+      </c>
       <c r="P11" s="6"/>
     </row>
   </sheetData>
@@ -2250,13 +2274,13 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A9:K9 M9:P9">
-    <cfRule type="expression" dxfId="14" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
       <formula>($J9="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>($J9="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>($J9="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Thêm các file phiên bản UC, cập nhật phiên bản UC 1.3, chuẩn bị gửi thầy.
</commit_message>
<xml_diff>
--- a/Docs/Q&A/DD_RFID_Q&A_v1.0.xlsx
+++ b/Docs/Q&A/DD_RFID_Q&A_v1.0.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
   <si>
     <t>Notes</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -703,13 +703,30 @@
       <t>the answer is available but not fully satisfied</t>
     </r>
   </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Tùy ý.</t>
+  </si>
+  <si>
+    <t>Tùy ý. Chỉ cần chạy tốt</t>
+  </si>
+  <si>
+    <t>Được</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ds vắng tức là có tên phải dự sự kiện (nếu bắt buộc thì tất cả hoặc đăng kí tư nguyện thì phải đi, không đi kể vắng)
+Ds phair tham dự là có trước, đi dự sẽ qẹt thẻ điểm danh, không có điểm danh là vắng
+Thầy Đệ
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
@@ -995,16 +1012,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1059,9 +1073,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1075,9 +1086,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1116,6 +1124,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1602,88 +1613,88 @@
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="32" t="s">
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="32" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="32" t="s">
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1723,246 +1734,246 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="66" style="8" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="33.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="66" style="7" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="39"/>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="19"/>
-    </row>
-    <row r="4" spans="1:2" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B3" s="18"/>
+    </row>
+    <row r="4" spans="1:2" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="17" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:2" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="17" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1987,7 +1998,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2002,267 +2013,280 @@
     <col min="8" max="8" width="11.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="11" style="3" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="20" style="26" customWidth="1"/>
-    <col min="12" max="12" width="17" style="26" customWidth="1"/>
-    <col min="13" max="13" width="17" style="3" customWidth="1"/>
+    <col min="11" max="11" width="20" style="24" customWidth="1"/>
+    <col min="12" max="13" width="17" style="24" customWidth="1"/>
     <col min="14" max="15" width="20.42578125" style="3" customWidth="1"/>
     <col min="16" max="16" width="22.42578125" style="3" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="40"/>
       <c r="C1" s="3">
         <f>COUNTIF(J:J, "Open")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="3">
         <f>COUNTIF(J:J, "In progress")</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="3">
         <f>COUNTIF(J:J, "Closed")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="3">
         <f>COUNTIF(J:J, "Canceled")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="46"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="3">
         <f>SUM(C1:C4)</f>
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="K7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29">
+      <c r="A8" s="27">
         <v>1</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21" t="s">
+      <c r="H8" s="20"/>
+      <c r="I8" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="K8" s="28">
+      <c r="J8" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" s="26">
         <v>42925</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="26">
         <f>K8+7</f>
         <v>42932</v>
       </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="21" t="s">
+      <c r="M8" s="26">
+        <v>42927</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="P8" s="6"/>
+      <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29">
+      <c r="A9" s="27">
         <v>2</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="21" t="s">
+      <c r="F9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21" t="s">
+      <c r="H9" s="20"/>
+      <c r="I9" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" s="28">
+      <c r="J9" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="26">
         <v>42925</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="26">
         <f t="shared" ref="L9:L11" si="0">K9+7</f>
         <v>42932</v>
       </c>
-      <c r="M9" s="25"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="21" t="s">
+      <c r="M9" s="26">
+        <v>42927</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="P9" s="6"/>
+      <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:16" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29">
+      <c r="A10" s="27">
         <v>3</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="29" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29" t="s">
+      <c r="H10" s="27"/>
+      <c r="I10" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="29" t="s">
+      <c r="J10" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="K10" s="30">
+      <c r="K10" s="28">
         <v>42925</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="26">
         <f t="shared" si="0"/>
         <v>42932</v>
       </c>
-      <c r="M10" s="31"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="29" t="s">
+      <c r="M10" s="28"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29">
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="27">
         <v>4</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="29" t="s">
+      <c r="F11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29" t="s">
+      <c r="H11" s="27"/>
+      <c r="I11" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" s="30">
+      <c r="J11" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" s="28">
         <v>42925</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="28">
         <f t="shared" si="0"/>
         <v>42932</v>
       </c>
-      <c r="M11" s="31"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="29" t="s">
+      <c r="M11" s="28">
+        <v>42927</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="P11" s="6"/>
+      <c r="P11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update Q&A, Xuất ra bằng excel
</commit_message>
<xml_diff>
--- a/Docs/Q&A/DD_RFID_Q&A_v1.0.xlsx
+++ b/Docs/Q&A/DD_RFID_Q&A_v1.0.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t>Notes</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -634,9 +634,6 @@
     <t>Danh sách vắng (không có vào theo toàn thể danh sách SV/CB) có phải là danh sách những người không đăng kí tham gia không?</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <r>
       <t>Open:</t>
     </r>
@@ -720,6 +717,9 @@
 Ds phair tham dự là có trước, đi dự sẽ qẹt thẻ điểm danh, không có điểm danh là vắng
 Thầy Đệ
 </t>
+  </si>
+  <si>
+    <t>excel</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -1073,20 +1073,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1124,9 +1127,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1613,78 +1613,78 @@
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="29" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="29" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="29" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="21"/>
@@ -1741,10 +1741,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="40"/>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1926,7 +1926,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1997,8 +1997,8 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2021,50 +2021,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="3">
         <f>COUNTIF(J:J, "Open")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="42"/>
       <c r="C2" s="3">
         <f>COUNTIF(J:J, "In progress")</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="42"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="3">
         <f>COUNTIF(J:J, "Closed")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="42"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="3">
         <f>COUNTIF(J:J, "Canceled")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="43"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="3">
         <f>SUM(C1:C4)</f>
         <v>4</v>
@@ -2107,7 +2107,7 @@
       <c r="L7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="44" t="s">
+      <c r="M7" s="29" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="4" t="s">
@@ -2135,7 +2135,7 @@
         <v>76</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>72</v>
@@ -2145,7 +2145,7 @@
         <v>77</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K8" s="26">
         <v>42925</v>
@@ -2158,7 +2158,7 @@
         <v>42927</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O8" s="20" t="s">
         <v>79</v>
@@ -2180,7 +2180,7 @@
         <v>84</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>72</v>
@@ -2190,7 +2190,7 @@
         <v>78</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9" s="26">
         <v>42925</v>
@@ -2222,7 +2222,9 @@
       <c r="E10" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="G10" s="27" t="s">
         <v>72</v>
       </c>
@@ -2231,7 +2233,7 @@
         <v>78</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K10" s="28">
         <v>42925</v>
@@ -2260,7 +2262,7 @@
         <v>85</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" s="27" t="s">
         <v>72</v>
@@ -2270,7 +2272,7 @@
         <v>78</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K11" s="28">
         <v>42925</v>

</xml_diff>

<commit_message>
thêm câu hỏi giao diện nhiều tab
</commit_message>
<xml_diff>
--- a/Docs/Q&A/DD_RFID_Q&A_v1.0.xlsx
+++ b/Docs/Q&A/DD_RFID_Q&A_v1.0.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="96">
   <si>
     <t>Notes</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -704,22 +704,29 @@
     <t>Closed</t>
   </si>
   <si>
-    <t>Tùy ý.</t>
-  </si>
-  <si>
     <t>Tùy ý. Chỉ cần chạy tốt</t>
   </si>
   <si>
     <t>Được</t>
   </si>
   <si>
-    <t xml:space="preserve">Ds vắng tức là có tên phải dự sự kiện (nếu bắt buộc thì tất cả hoặc đăng kí tư nguyện thì phải đi, không đi kể vắng)
-Ds phair tham dự là có trước, đi dự sẽ qẹt thẻ điểm danh, không có điểm danh là vắng
-Thầy Đệ
-</t>
-  </si>
-  <si>
     <t>excel</t>
+  </si>
+  <si>
+    <t>Chức năng bổ sung</t>
+  </si>
+  <si>
+    <t>Muốn xây dựng giao diện quản trị theo dạng tab, khi chuyển tab không phải reset lại nội dung của tab trước.</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Ds vắng tức là có tên phải dự sự kiện (nếu bắt buộc thì tất cả hoặc đăng kí tư nguyện thì phải đi, không đi kể vắng)
+Ds phair tham dự là có trước, đi dự sẽ qẹt thẻ điểm danh, không có điểm danh là vắng</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1139,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1995,10 +2086,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2027,7 +2118,7 @@
       <c r="B1" s="41"/>
       <c r="C1" s="3">
         <f>COUNTIF(J:J, "Open")</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2067,7 +2158,7 @@
       <c r="B5" s="44"/>
       <c r="C5" s="3">
         <f>SUM(C1:C4)</f>
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2135,7 +2226,7 @@
         <v>76</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>72</v>
@@ -2157,9 +2248,7 @@
       <c r="M8" s="26">
         <v>42927</v>
       </c>
-      <c r="N8" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="N8" s="5"/>
       <c r="O8" s="20" t="s">
         <v>79</v>
       </c>
@@ -2180,7 +2269,7 @@
         <v>84</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>72</v>
@@ -2223,7 +2312,7 @@
         <v>83</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G10" s="27" t="s">
         <v>72</v>
@@ -2236,11 +2325,11 @@
         <v>87</v>
       </c>
       <c r="K10" s="28">
-        <v>42925</v>
+        <v>42926</v>
       </c>
       <c r="L10" s="26">
-        <f t="shared" si="0"/>
-        <v>42932</v>
+        <f>K10+7</f>
+        <v>42933</v>
       </c>
       <c r="M10" s="28"/>
       <c r="N10" s="5"/>
@@ -2249,7 +2338,7 @@
       </c>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:16" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="27">
         <v>4</v>
       </c>
@@ -2262,7 +2351,7 @@
         <v>85</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G11" s="27" t="s">
         <v>72</v>
@@ -2275,11 +2364,11 @@
         <v>87</v>
       </c>
       <c r="K11" s="28">
-        <v>42925</v>
+        <v>42926</v>
       </c>
       <c r="L11" s="28">
-        <f t="shared" si="0"/>
-        <v>42932</v>
+        <f>K11+7</f>
+        <v>42933</v>
       </c>
       <c r="M11" s="28">
         <v>42927</v>
@@ -2289,6 +2378,409 @@
         <v>79</v>
       </c>
       <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="27">
+        <v>5</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K12" s="28">
+        <v>42928</v>
+      </c>
+      <c r="L12" s="28">
+        <f>K12+7</f>
+        <v>42935</v>
+      </c>
+      <c r="M12" s="28"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="27">
+        <v>6</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="27">
+        <v>7</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="27">
+        <v>8</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="27">
+        <v>9</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="27">
+        <v>10</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="27">
+        <v>11</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="27">
+        <v>12</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="27">
+        <v>13</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="27">
+        <v>14</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="27">
+        <v>15</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P22" s="5"/>
+    </row>
+    <row r="23" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="27">
+        <v>16</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="27">
+        <v>17</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="27">
+        <v>18</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P25" s="5"/>
+    </row>
+    <row r="26" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="27">
+        <v>19</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2299,61 +2791,83 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="A9:K9 M9:P9">
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="A9 M9:P9 C9:K9">
+    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
       <formula>($J9="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="17" stopIfTrue="1">
       <formula>($J9="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="18" stopIfTrue="1">
       <formula>($J9="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:K10 M10:P10">
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+  <conditionalFormatting sqref="A10 M10:P10 C10:K10">
+    <cfRule type="expression" dxfId="20" priority="13" stopIfTrue="1">
       <formula>($J10="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="14" stopIfTrue="1">
       <formula>($J10="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="15" stopIfTrue="1">
       <formula>($J10="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:K11 M11:P11">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="A11 M11:P11 A13 A15 A17 A19 A21 A23 A25 J12:J26 O12:O26 C11:K11">
+    <cfRule type="expression" dxfId="17" priority="10" stopIfTrue="1">
       <formula>($J11="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="11" stopIfTrue="1">
       <formula>($J11="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="12" stopIfTrue="1">
       <formula>($J11="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:P8 L9:L11">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A8:P8 L9:L11 B9:B26">
+    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
       <formula>($J8="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="8" stopIfTrue="1">
       <formula>($J8="Closed")</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="12" priority="9" stopIfTrue="1">
+      <formula>($J8="Canceled")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12 M12:N26 A14 A16 A18 A20 A22 A24 A26 K12:K26 P12:P26 C12:I26">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+      <formula>($J12="In Progress")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>($J12="Closed")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+      <formula>($J12="Canceled")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12:L26">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>($J12="In Progress")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>($J12="Closed")</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>($J8="Canceled")</formula>
+      <formula>($J12="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I11">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O8:O11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O8:O26">
       <formula1>"Clarification,Confirmation,HSK Defect"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J26">
       <formula1>"Open,In progress,Closed,Canceled"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B26">
       <formula1>"Requirement,Design,Coding,Test,Deployment,Project management"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>